<commit_message>
Timestamp auf Datum umgestellt
</commit_message>
<xml_diff>
--- a/WEBINP_Wanderplan_PWV_Speyer_aktuell.xlsx
+++ b/WEBINP_Wanderplan_PWV_Speyer_aktuell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d003388/dev/git/wanderplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D65218-E702-0648-8D0E-9E033AA2886E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AD2A2C-505D-DD47-9F88-E63689B1AFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="26560" xr2:uid="{AA1FAD4D-075F-4CA5-ADA8-0B73289FDBD1}"/>
   </bookViews>
@@ -1142,10 +1142,10 @@
   <dimension ref="A1:M79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Refaktoring und kleinere Anpassungen
</commit_message>
<xml_diff>
--- a/WEBINP_Wanderplan_PWV_Speyer_aktuell.xlsx
+++ b/WEBINP_Wanderplan_PWV_Speyer_aktuell.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernh\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E222E69A-315A-46E9-9480-2F5E76F90A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75C7979E-37C6-43AD-A76C-1B740E79B1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7504F714-6F17-4CAE-9A03-5A4D375E8B13}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{09DFD5FF-5895-4491-A38B-F6FB9CF35099}"/>
   </bookViews>
   <sheets>
     <sheet name="WEBINP" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="227">
   <si>
     <t>Datum</t>
   </si>
@@ -269,6 +269,9 @@
     <t>20220320_MON_Leistadt, v4.pdf</t>
   </si>
   <si>
+    <t>wanderbericht/monatswanderung-leistadt/</t>
+  </si>
+  <si>
     <t>Familienwanderung auf die Hohe Loog</t>
   </si>
   <si>
@@ -341,18 +344,12 @@
     <t>Wanderführer-Stammtisch</t>
   </si>
   <si>
-    <t xml:space="preserve">Treffpunkt: 17:30 Uhr Vereinsheim Skiclub Speyer. </t>
-  </si>
-  <si>
     <t>Familienwanderung am Hüttenbrunnen</t>
   </si>
   <si>
     <t xml:space="preserve">Die ursprünglich geplante Nachtwanderung im Auwald kann leider nicht stattfinden.&lt;br&gt;ca. 7 km. </t>
   </si>
   <si>
-    <t xml:space="preserve">Treffpunkt: 13:00 Uhr am Parkplatz Stadthalle Speyer. &lt;br&gt;Anmeldefrist: 28.04.2022. </t>
-  </si>
-  <si>
     <t>20220430_FAM_Huettenbrunnen.pdf</t>
   </si>
   <si>
@@ -362,25 +359,21 @@
     <t xml:space="preserve">ca. 19 km, ca. 500 HM. </t>
   </si>
   <si>
-    <t xml:space="preserve">Treffpunkt: 08:30 Uhr am Parkplatz Stadthalle Speyer
-Zustieg Parkplatz Bad Dürkheim um 09:15 Uhr möglich. &lt;br&gt;Anmeldefrist: 27.04.2022. </t>
-  </si>
-  <si>
     <t>Andreas Steffen&lt;br&gt;Peter Hohmann</t>
   </si>
   <si>
     <t>20220501_SPW_Weinsteig, Etappe 2.pdf</t>
   </si>
   <si>
+    <t>wanderbericht/sportwanderung-weinsteig-2-von-neuleiningen-nach-bad-duerkheim-01-05-2022/</t>
+  </si>
+  <si>
     <t>Ausflug in den Sichtungsgarten Weinheim</t>
   </si>
   <si>
     <t>ca. 5 km. FFP2-Maskenpflicht im ÖPNV</t>
   </si>
   <si>
-    <t xml:space="preserve">Treffpunkt: 09:45 Uhr, Vorhalle HBF Speyer. &lt;br&gt;Anmeldefrist: 02.05.2022. </t>
-  </si>
-  <si>
     <t>20220504_SEN_Sichtungsgarten.pdf</t>
   </si>
   <si>
@@ -393,9 +386,6 @@
     <t xml:space="preserve">ca. 7 km. </t>
   </si>
   <si>
-    <t xml:space="preserve">Treffpunkt: 17:30 Uhr, Parkplatz Kletterwald. &lt;br&gt;Anmeldefrist: 03.05.2022, max. 12 Teilnehmer. </t>
-  </si>
-  <si>
     <t>Peter Hohmann</t>
   </si>
   <si>
@@ -411,9 +401,6 @@
     <t xml:space="preserve">ca. 60 km. </t>
   </si>
   <si>
-    <t xml:space="preserve">Treffpunkt: 09:30 Uhr, Denkmal „Die Welle“, Rheinpromenade. &lt;br&gt;Anmeldefrist: 05.05.2022, max. 20 Teilnehmer. </t>
-  </si>
-  <si>
     <t>20220508_RAD_Speyerbach.pdf</t>
   </si>
   <si>
@@ -421,9 +408,6 @@
   </si>
   <si>
     <t>in Zusammenarbeit mit dem Vogelschutzverein Hanhofen.&lt;br&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treffpunkt: 13:45 Uhr, Vereinsheim der Vogelfreunde Hanhofen in Hanhofen. &lt;br&gt;Anmeldefrist: 10.05.2022. </t>
   </si>
   <si>
     <t>Bernhard Steigleider, Helmut Back</t>
@@ -448,19 +432,49 @@
     <t>20220518_JSW_Kollerinsel.pdf</t>
   </si>
   <si>
+    <t xml:space="preserve">Treffpunkt: 17:30 Uhr, Parkplatz Kletterwald. &lt;br&gt;Anmeldefrist: 03.05.2022, max. 12 Teilnehmer. </t>
+  </si>
+  <si>
     <t>Auf den Spuren der Treidler in Hördt am Rhein</t>
   </si>
   <si>
     <t>LW: ca. 13 km, KW: ca. 8 km.</t>
   </si>
   <si>
+    <t xml:space="preserve">Treffpunkt: ab 09:00 Uhr an den üblichen Bushaltestellen. &lt;br&gt;Anmeldefrist: 21.05.2022, max 50 Teilnehmer. </t>
+  </si>
+  <si>
+    <t>Bernhard Steigleider, Dr. Rik Naus</t>
+  </si>
+  <si>
+    <t>Matthias Brunnmüller, Rudi Waldinger (PWV Hördt)</t>
+  </si>
+  <si>
+    <t>20220522_MON_Treidlerweg.pdf</t>
+  </si>
+  <si>
     <t>Schorlewanderung bei Deidesheim</t>
   </si>
   <si>
+    <t>ca. 7 km. FFP2-Maskenpflicht im ÖPNV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treffpunkt: 10:45 Uhr, Vorhalle HBF Speyer. &lt;br&gt;Anmeldefrist: 26.05.2022. </t>
+  </si>
+  <si>
+    <t>20220528_FUN_Schorlewanderung_V2.pdf</t>
+  </si>
+  <si>
     <t>Pfälzer Weinsteig, Etappe 3, von Bad Dürkheim nach Deidesheim</t>
   </si>
   <si>
-    <t xml:space="preserve">ca. 15 km, ca. 500 HM. </t>
+    <t>ca. 15 km, ca. 500 HM. FFP2-Maskenpflicht im ÖPNV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treffpunkt: 08:45 Uhr, Vorhalle HBF Speyer. &lt;br&gt;Anmeldefrist: 02.06.2022. </t>
+  </si>
+  <si>
+    <t>20220604_SPW_Weinsteig_Etappe_3.pdf</t>
   </si>
   <si>
     <t>Ausflug auf das Hambacher Schloss mit Zeter Berghaus</t>
@@ -469,9 +483,6 @@
     <t xml:space="preserve">ca. 5 km. </t>
   </si>
   <si>
-    <t xml:space="preserve"> N. N.</t>
-  </si>
-  <si>
     <t>Mitgliederversammlung (Nachholtermin)</t>
   </si>
   <si>
@@ -493,9 +504,15 @@
     <t>Kinderspaß im Modenbachtal</t>
   </si>
   <si>
+    <t xml:space="preserve">Treffpunkt: 11:00 Uhr, Stadthalle Speyer. &lt;br&gt;Anmeldefrist: 16.06.2022. </t>
+  </si>
+  <si>
     <t>Sebastian Bittmann</t>
   </si>
   <si>
+    <t>20220619_FAM_Modenbachtal.pdf</t>
+  </si>
+  <si>
     <t>Über Dudenhofen, Schifferstadt nach Waldsee und zurück</t>
   </si>
   <si>
@@ -505,6 +522,15 @@
     <t>Wolfgang Laser</t>
   </si>
   <si>
+    <t>Sportliche Radwanderung von Speyer über Mussbach nach Deidesheim und zurück</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca. 56 km. </t>
+  </si>
+  <si>
+    <t>Marcus Homa, Helmut Back</t>
+  </si>
+  <si>
     <t>Barfußwandern auf die Rietburg mit der OG Landau</t>
   </si>
   <si>
@@ -520,15 +546,22 @@
     <t xml:space="preserve">Treffpunkt: 17:00 Uhr, Am Domnapf. </t>
   </si>
   <si>
-    <t>Sa / So
-02.07.2022
-03.07.2022</t>
+    <t>Sa / So&lt;br&gt;02.07.2022&lt;br&gt;03.07.2022</t>
   </si>
   <si>
     <t>Der komplette Rodalbener Felsenwanderweg</t>
   </si>
   <si>
-    <t xml:space="preserve">mit Übernachtung auf dem Hilschberghaus.&lt;br&gt;ca. 23 km je Tag, ca. 500 HM. </t>
+    <t xml:space="preserve">mit Übernachtung auf dem Hilschberghaus..&lt;br&gt;ca. 23 km je Tag, ca. 500 HM. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmeldefrist: 18.05.2022. </t>
+  </si>
+  <si>
+    <t>20220702_SPW_Rodalben_VORANKUENDIGUNG.pdf</t>
+  </si>
+  <si>
+    <t>Übernachtungswunsch: ________(Doppel/Dreifach/Einzelzimmer)</t>
   </si>
   <si>
     <t>Auf dem Felsenwanderweg in Rodalben</t>
@@ -540,15 +573,19 @@
     <t xml:space="preserve">ca. 40 km. </t>
   </si>
   <si>
-    <t>Fr-So
-15.-17.
-07.2022</t>
+    <t>Fr-So&lt;br&gt;15.-17.&lt;br&gt;07.2022</t>
   </si>
   <si>
     <t>Familienwochenende im Hochschwarzwald</t>
   </si>
   <si>
     <t>in der JH Todtnauberg mit 2 Übernachtungen.&lt;br&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmeldefrist: 09.06.2022. </t>
+  </si>
+  <si>
+    <t>20220715_FAM_Todtnauberg.pdf</t>
   </si>
   <si>
     <t>Zum Schifferstadter Mittellacheweiher</t>
@@ -725,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -741,9 +778,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1204,15 +1238,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA205AA-10E2-47AA-B3BF-6AC2DCED95DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB255A1-6C92-48F2-848B-53EFDC97120D}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:N78"/>
+  <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1618,6 +1652,9 @@
         <v>74</v>
       </c>
       <c r="L17" s="5"/>
+      <c r="N17" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
@@ -1627,16 +1664,16 @@
         <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>54</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L18" s="5">
         <v>44642</v>
@@ -1650,10 +1687,10 @@
         <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>16</v>
@@ -1668,22 +1705,22 @@
         <v>34</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>37</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L20" s="5">
         <v>44651</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -1694,16 +1731,16 @@
         <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L21" s="5">
         <v>44655</v>
@@ -1717,25 +1754,25 @@
         <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L22" s="5">
         <v>44657</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -1746,25 +1783,25 @@
         <v>29</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L23" s="5">
         <v>44669</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>44680</v>
       </c>
@@ -1772,9 +1809,6 @@
         <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F24" s="2" t="s">
         <v>99</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -1782,7 +1816,7 @@
       </c>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>44681</v>
       </c>
@@ -1795,23 +1829,20 @@
       <c r="E25" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="G25" s="3" t="s">
         <v>54</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L25" s="5">
         <v>44679</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>44682</v>
       </c>
@@ -1819,28 +1850,28 @@
         <v>34</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="G26" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="I26" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="L26" s="5">
         <v>44678</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>44685</v>
       </c>
@@ -1848,28 +1879,25 @@
         <v>39</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L27" s="5">
         <v>44683</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>44686</v>
       </c>
@@ -1877,51 +1905,45 @@
         <v>68</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="I28" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="L28" s="5">
         <v>44684</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>44689</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="L29" s="5">
         <v>44686</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>44693</v>
       </c>
@@ -1929,22 +1951,19 @@
         <v>68</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="I30" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L30" s="5">
         <v>44684</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>44695</v>
       </c>
@@ -1952,19 +1971,16 @@
         <v>24</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L31" s="5">
         <v>44691</v>
@@ -1978,25 +1994,25 @@
         <v>29</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L32" s="5">
         <v>44697</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>44700</v>
       </c>
@@ -2004,25 +2020,25 @@
         <v>68</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="I33" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="L33" s="5">
         <v>44684</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>44703</v>
       </c>
@@ -2030,20 +2046,28 @@
         <v>18</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="I34" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L34" s="5"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L34" s="5">
+        <v>44702</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>44709</v>
       </c>
@@ -2053,12 +2077,23 @@
       <c r="D35" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="E35" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="G35" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L35" s="5"/>
-    </row>
-    <row r="36" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I35" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="L35" s="5">
+        <v>44707</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>44716</v>
       </c>
@@ -2066,17 +2101,25 @@
         <v>34</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L36" s="5"/>
-    </row>
-    <row r="37" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I36" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="L36" s="5">
+        <v>44714</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>44720</v>
       </c>
@@ -2084,17 +2127,17 @@
         <v>39</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>44722</v>
       </c>
@@ -2102,17 +2145,17 @@
         <v>14</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>16</v>
       </c>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>44724</v>
       </c>
@@ -2120,17 +2163,17 @@
         <v>18</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>44727</v>
       </c>
@@ -2138,17 +2181,17 @@
         <v>29</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>44731</v>
       </c>
@@ -2156,295 +2199,325 @@
         <v>24</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="L41" s="5"/>
-    </row>
-    <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="L41" s="5">
+        <v>44728</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>44734</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
+        <v>44737</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
         <v>44738</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L43" s="5"/>
-    </row>
-    <row r="44" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
+      <c r="D44" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
         <v>44742</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G44" s="3" t="s">
+      <c r="C45" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L44" s="5"/>
-    </row>
-    <row r="45" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
+      <c r="L45" s="5"/>
+    </row>
+    <row r="46" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
         <v>44744</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L45" s="5"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
-        <v>44745</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>145</v>
+        <v>169</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L46" s="5"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I46" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L46" s="5">
+        <v>44699</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
+        <v>44745</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L47" s="5"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
         <v>44751</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G47" s="3" t="s">
+      <c r="C48" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L47" s="5"/>
-    </row>
-    <row r="48" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
+      <c r="L48" s="5"/>
+    </row>
+    <row r="49" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
         <v>44757</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="B49" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="G48" s="3" t="s">
+      <c r="D49" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L48" s="5"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="4">
+      <c r="I49" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="L49" s="5">
+        <v>44721</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
         <v>44762</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="L49" s="5"/>
-    </row>
-    <row r="50" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="4">
-        <v>44766</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="D50" s="2" t="s">
-        <v>169</v>
+        <v>181</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>117</v>
+        <v>182</v>
       </c>
       <c r="L50" s="5"/>
     </row>
     <row r="51" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
+        <v>44766</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L51" s="5"/>
+    </row>
+    <row r="52" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="4">
         <v>44780</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G51" s="3" t="s">
+      <c r="D52" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="L51" s="5"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="4">
-        <v>44783</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="L52" s="5"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
-        <v>44794</v>
+        <v>44783</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="H53" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L53" s="5"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
+        <v>44794</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L54" s="5"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="4">
         <v>44797</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="L54" s="5"/>
-    </row>
-    <row r="55" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="4">
+      <c r="D55" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L55" s="5"/>
+    </row>
+    <row r="56" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="4">
         <v>44808</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G55" s="3" t="s">
+      <c r="D56" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="L55" s="5"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="4">
-        <v>44811</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
-        <v>44815</v>
+        <v>44811</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>180</v>
+        <v>193</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="L57" s="5"/>
     </row>
@@ -2453,154 +2526,154 @@
         <v>44815</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
+        <v>44815</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L59" s="5"/>
+    </row>
+    <row r="60" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="4">
         <v>44822</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="G59" s="3" t="s">
+      <c r="D60" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="L59" s="5"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="4">
-        <v>44825</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
+        <v>44825</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="L61" s="5"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62" s="4">
         <v>44829</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G61" s="3" t="s">
+      <c r="D62" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G62" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L61" s="5"/>
-    </row>
-    <row r="62" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="4">
+      <c r="L62" s="5"/>
+    </row>
+    <row r="63" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="4">
         <v>44835</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G62" s="3" t="s">
+      <c r="D63" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G63" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L62" s="5"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="4">
+      <c r="L63" s="5"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64" s="4">
         <v>44839</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G63" s="3" t="s">
+      <c r="D64" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G64" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L63" s="5"/>
-    </row>
-    <row r="64" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A64" s="4">
+      <c r="L64" s="5"/>
+    </row>
+    <row r="65" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A65" s="4">
         <v>44841</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G64" s="3" t="s">
+      <c r="D65" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G65" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="L64" s="5"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="4">
-        <v>44853</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="L65" s="5"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
-        <v>44857</v>
+        <v>44853</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>54</v>
+        <v>198</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="L66" s="5"/>
     </row>
@@ -2609,210 +2682,225 @@
         <v>44857</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L67" s="5"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A68" s="4">
+        <v>44857</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L67" s="5"/>
-    </row>
-    <row r="68" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="4">
+      <c r="D68" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="L68" s="5"/>
+    </row>
+    <row r="69" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="4">
         <v>44864</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G68" s="3" t="s">
+      <c r="D69" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G69" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L68" s="5"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A69" s="4">
+      <c r="L69" s="5"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" s="4">
         <v>44865</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D70" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L70" s="5"/>
+    </row>
+    <row r="71" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="4">
+        <v>44869</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L71" s="5"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A72" s="4">
+        <v>44871</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L72" s="5"/>
+    </row>
+    <row r="73" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A73" s="4">
+        <v>44874</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L73" s="5"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A74" s="4">
+        <v>44884</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="L74" s="5"/>
+    </row>
+    <row r="75" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="4">
+        <v>44885</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="L75" s="5"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76" s="4">
+        <v>44888</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="G69" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L69" s="5"/>
-    </row>
-    <row r="70" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="4">
-        <v>44869</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="E76" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="L76" s="5"/>
+    </row>
+    <row r="77" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A77" s="4">
+        <v>44898</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G70" s="3" t="s">
+      <c r="D77" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G77" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="L70" s="5"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A71" s="4">
-        <v>44871</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L71" s="5"/>
-    </row>
-    <row r="72" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="4">
-        <v>44874</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L72" s="5"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A73" s="4">
-        <v>44884</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="L73" s="5"/>
-    </row>
-    <row r="74" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="4">
-        <v>44885</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L74" s="5"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A75" s="4">
-        <v>44888</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="L75" s="5"/>
-    </row>
-    <row r="76" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="4">
-        <v>44898</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L76" s="5"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A77" s="4">
-        <v>44901</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="L77" s="5"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
-        <v>44902</v>
+        <v>44901</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L78" s="5"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79" s="4">
+        <v>44902</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L79" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{BF1F9378-5A8B-46DE-BD61-4544C985A387}"/>

</xml_diff>

<commit_message>
Keine Anmeldung für abgesagte Termine
</commit_message>
<xml_diff>
--- a/WEBINP_Wanderplan_PWV_Speyer_aktuell.xlsx
+++ b/WEBINP_Wanderplan_PWV_Speyer_aktuell.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernh\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75C7979E-37C6-43AD-A76C-1B740E79B1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9839C420-5B8E-47DB-9CFB-5E97452FD4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{09DFD5FF-5895-4491-A38B-F6FB9CF35099}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4B7CC834-4843-48B2-A415-50A3D666B0A2}"/>
   </bookViews>
   <sheets>
     <sheet name="WEBINP" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="241">
   <si>
     <t>Datum</t>
   </si>
@@ -56,10 +56,10 @@
     <t>Veranstaltung</t>
   </si>
   <si>
-    <t xml:space="preserve">Veranstaltung 2 </t>
-  </si>
-  <si>
-    <t>Veranstaltung 3</t>
+    <t>Veranstaltung2</t>
+  </si>
+  <si>
+    <t>Veranstaltung3</t>
   </si>
   <si>
     <t>WF</t>
@@ -104,7 +104,7 @@
     <t>Glühweinwanderung im Speyerer Stadtwald</t>
   </si>
   <si>
-    <t>LW: ca. 13 km, KW: ca. 4 km.Teilnahme unter 2G-Plus. Wir wandern in 10er-Gruppen.</t>
+    <t>LW: ca. 13 km, KW: ca. 4 km. Teilnahme unter 2G-Plus. Wir wandern in 10er-Gruppen.</t>
   </si>
   <si>
     <t>Nicola Schmidt-Geheb</t>
@@ -137,7 +137,7 @@
     <t>Jungseniorenwanderung ins Kaltenbrunner Tal</t>
   </si>
   <si>
-    <t>11 km. Teilnahme unter 2G-Plus. Wir wandern in 10er-Gruppen.</t>
+    <t>ca.11 km. Teilnahme unter 2G-Plus. Wir wandern in 10er-Gruppen.</t>
   </si>
   <si>
     <t>Bernhard Steigleider</t>
@@ -191,7 +191,7 @@
     <t>Auf dem Druslach-Bacherlebnisweg von Lingenfeld nach Zeiskam</t>
   </si>
   <si>
-    <t>12 km. Teilnahme unter 2G-Plus. Wir wandern in 10er-Gruppen.</t>
+    <t>ca.12 km. Teilnahme unter 2G-Plus. Wir wandern in 10er-Gruppen.</t>
   </si>
   <si>
     <t>20220216_JSW_Druslach.pdf</t>
@@ -200,7 +200,7 @@
     <t>Durch den Bienwald auf den Spuren des Westwalls</t>
   </si>
   <si>
-    <t>LW: ca. 9 km, KW: ca. 6 km.Teilnahme unter 2G-Plus.</t>
+    <t>LW: ca. 9 km, KW: ca. 6 km. Teilnahme unter 2G-Plus.</t>
   </si>
   <si>
     <t>Tom Meigen</t>
@@ -242,7 +242,7 @@
     <t>Rund um die Insel Elisabethenwörth</t>
   </si>
   <si>
-    <t>10 km. Teilnahme unter 2G.</t>
+    <t>ca.10 km. Teilnahme unter 2G.</t>
   </si>
   <si>
     <t>20220216_JSW_Elisabethenwoerth, v1.pdf</t>
@@ -263,7 +263,7 @@
     <t>Römer, Grafen, Ungeheuer und der Teufel im Forst Ganerben bei Leistadt</t>
   </si>
   <si>
-    <t>LW: ca. 11 km, KW: ca. 5 km.Teilnahme unter 2G.</t>
+    <t>LW: ca. 11 km, KW: ca. 5 km. Teilnahme unter 2G.</t>
   </si>
   <si>
     <t>20220320_MON_Leistadt, v4.pdf</t>
@@ -284,7 +284,7 @@
     <t>Monatstreffen April</t>
   </si>
   <si>
-    <t>u. a. Vortrag zu den Rittersteinen im Pfälzerwald.&lt;br&gt;</t>
+    <t>u. a. Vortrag zu den Rittersteinen im Pfälzerwald.</t>
   </si>
   <si>
     <t>Lug – Geiersteine und Höllenberg: Felslandschaften zum Staunen</t>
@@ -311,10 +311,10 @@
     <t>Vom Wasserhaus Harthausen zum Waldhaus Gommersheim und zurück</t>
   </si>
   <si>
-    <t>Die ursprünglich geplante Dünenwanderung in Speyer mit der OG Bad Dürkheim findet nicht statt.&lt;br&gt;LW: ca. 9 km, KW: ca. 5 km.</t>
-  </si>
-  <si>
-    <t>Helmut Back, Dr. Rik Naus</t>
+    <t xml:space="preserve">Die ursprünglich geplante Dünenwanderung in Speyer mit der OG Bad Dürkheim findet nicht statt.&lt;br&gt;LW: ca. 9 km, KW: ca. 5 km. </t>
+  </si>
+  <si>
+    <t>Helmut Back&lt;br&gt;Dr. Rik Naus</t>
   </si>
   <si>
     <t>Dr. Lina Seidel</t>
@@ -329,7 +329,7 @@
     <t>Auf die Insel Flotzgrün</t>
   </si>
   <si>
-    <t xml:space="preserve">12 km. </t>
+    <t xml:space="preserve">ca.12 km. </t>
   </si>
   <si>
     <t>Dr. Rik Naus</t>
@@ -407,10 +407,10 @@
     <t xml:space="preserve">Exkursion: „Besuch bei den Vögeln im Allmendwald“ </t>
   </si>
   <si>
-    <t>in Zusammenarbeit mit dem Vogelschutzverein Hanhofen.&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>Bernhard Steigleider, Helmut Back</t>
+    <t>in Zusammenarbeit mit dem Vogelschutzverein Hanhofen.</t>
+  </si>
+  <si>
+    <t>Bernhard Steigleider&lt;br&gt;Helmut Back</t>
   </si>
   <si>
     <t>20220430_FAM_Allmendwald.pdf</t>
@@ -419,35 +419,25 @@
     <t>Rund um die Kollerinsel</t>
   </si>
   <si>
-    <t xml:space="preserve">10 km. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treffpunkt: 10:00 Uhr am Parkplatz Stadthalle Speyer
-Zustieg an der Kollerfähre um 10:20 Uhr möglich. &lt;br&gt;Anmeldefrist: 16.05.2022. </t>
-  </si>
-  <si>
-    <t>Helga Peters, Waltraud Schimpf</t>
+    <t xml:space="preserve">ca.10 km. </t>
+  </si>
+  <si>
+    <t>Helga Peters&lt;br&gt;Waltraud Schimpf</t>
   </si>
   <si>
     <t>20220518_JSW_Kollerinsel.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">Treffpunkt: 17:30 Uhr, Parkplatz Kletterwald. &lt;br&gt;Anmeldefrist: 03.05.2022, max. 12 Teilnehmer. </t>
-  </si>
-  <si>
     <t>Auf den Spuren der Treidler in Hördt am Rhein</t>
   </si>
   <si>
-    <t>LW: ca. 13 km, KW: ca. 8 km.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treffpunkt: ab 09:00 Uhr an den üblichen Bushaltestellen. &lt;br&gt;Anmeldefrist: 21.05.2022, max 50 Teilnehmer. </t>
-  </si>
-  <si>
-    <t>Bernhard Steigleider, Dr. Rik Naus</t>
-  </si>
-  <si>
-    <t>Matthias Brunnmüller, Rudi Waldinger (PWV Hördt)</t>
+    <t xml:space="preserve">LW: ca. 13 km, KW: ca. 8 km. </t>
+  </si>
+  <si>
+    <t>Bernhard Steigleider&lt;br&gt;Dr. Rik Naus</t>
+  </si>
+  <si>
+    <t>Matthias Brunnmüller&lt;br&gt;Rudi Waldinger (PWV Hördt)</t>
   </si>
   <si>
     <t>20220522_MON_Treidlerweg.pdf</t>
@@ -459,213 +449,264 @@
     <t>ca. 7 km. FFP2-Maskenpflicht im ÖPNV</t>
   </si>
   <si>
-    <t xml:space="preserve">Treffpunkt: 10:45 Uhr, Vorhalle HBF Speyer. &lt;br&gt;Anmeldefrist: 26.05.2022. </t>
-  </si>
-  <si>
     <t>20220528_FUN_Schorlewanderung_V2.pdf</t>
   </si>
   <si>
+    <t>Jobticket/Karte Ü60/9€-Ticket vorhanden: ________</t>
+  </si>
+  <si>
+    <t>wanderbericht/schorlewanderung-bei-deidesheim-28-mai-2022/</t>
+  </si>
+  <si>
     <t>Pfälzer Weinsteig, Etappe 3, von Bad Dürkheim nach Deidesheim</t>
   </si>
   <si>
     <t>ca. 15 km, ca. 500 HM. FFP2-Maskenpflicht im ÖPNV</t>
   </si>
   <si>
-    <t xml:space="preserve">Treffpunkt: 08:45 Uhr, Vorhalle HBF Speyer. &lt;br&gt;Anmeldefrist: 02.06.2022. </t>
-  </si>
-  <si>
     <t>20220604_SPW_Weinsteig_Etappe_3.pdf</t>
   </si>
   <si>
     <t>Ausflug auf das Hambacher Schloss mit Zeter Berghaus</t>
   </si>
   <si>
+    <t>ca. 5 km. FFP2-Maskenpflicht im ÖPNV und im Hambacher Schloss</t>
+  </si>
+  <si>
+    <t>20220608_SEN_Hambacher_Schloss.pdf</t>
+  </si>
+  <si>
+    <t>Jobticket/Karte Ü60/9€-Ticket vorhanden: ________&lt;br&gt;Teilnahme an Führung (ja/nein): ______</t>
+  </si>
+  <si>
+    <t>Mitgliederversammlung (Nachholtermin)</t>
+  </si>
+  <si>
+    <t>Zur Rebenblüte durch die Deidesheimer Weinlagen mit 4-gängiger Weinverköstigung</t>
+  </si>
+  <si>
+    <t>Kosten EUR 25,00 für Mitglieder, EUR 28,00 für Gäste zzgl. EUR 6 EUR für Zugticket, falls notwendig.&lt;br&gt;LW: ca. 12 km, KW: ca. 7 km. FFP2-Maskenpflicht im ÖPNV</t>
+  </si>
+  <si>
+    <t>20220612_MON_Deidesheim_V2.pdf</t>
+  </si>
+  <si>
+    <t>Auf der Ketscher Insel</t>
+  </si>
+  <si>
+    <t>ca. 8 km Wanderung und ca. 22 km Radfahren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treffpunkt: 10:00 Uhr, Domnapf. &lt;br&gt;Anmeldung erwünscht bis 13.06.2022. </t>
+  </si>
+  <si>
+    <t>20220615_JSW_Ketscher_Insel.pdf</t>
+  </si>
+  <si>
+    <t>Kinderspaß im Modenbachtal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treffpunkt: 11:00 Uhr, Stadthalle Speyer. &lt;br&gt;Anmeldung erwünscht bis 16.06.2022. </t>
+  </si>
+  <si>
+    <t>Sebastian Bittmann</t>
+  </si>
+  <si>
+    <t>20220619_FAM_Modenbachtal.pdf</t>
+  </si>
+  <si>
+    <t>Über Dudenhofen, Schifferstadt nach Waldsee und zurück</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca. 28 km. </t>
+  </si>
+  <si>
+    <t>Wolfgang Laser</t>
+  </si>
+  <si>
+    <t>20220622_RAD_Waldsee.pdf</t>
+  </si>
+  <si>
+    <t>Sportliche Radwanderung von Speyer über Mussbach nach Deidesheim und zurück</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca. 55 km. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treffpunkt: 11:00 Uhr am Spielplatz ‚Am Woogbach‘ im Woogbachpark. &lt;br&gt;Anmeldung erwünscht bis 23.06.2022, max. 20 Teilnehmer. </t>
+  </si>
+  <si>
+    <t>Marcus Homa&lt;br&gt;Helmut Back</t>
+  </si>
+  <si>
+    <t>20220625_RAD_Deidesheim.pdf</t>
+  </si>
+  <si>
+    <t>Barfußwandern auf die Rietburg mit der OG Landau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca. 15 km. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treffpunkt: 9:15 Uhr Stadthalle Speyer. &lt;br&gt;Anmeldung erwünscht bis 23.06.2022. </t>
+  </si>
+  <si>
+    <t>20220626_FUN_Barfuß_Rietburg.pdf</t>
+  </si>
+  <si>
+    <t>RAD-B</t>
+  </si>
+  <si>
+    <t>Fahrrad-Feierabend-Tour über Binsfeld und Otterstadt ins Reffenthal und zurück</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treffpunkt: 17:00 Uhr, Domnapf. &lt;br&gt;Anmeldung erwünscht bis 28.06.2022. </t>
+  </si>
+  <si>
+    <t>20220630_RAD_Feierabend.pdf</t>
+  </si>
+  <si>
+    <t>Sa / So&lt;br&gt;02.07.2022&lt;br&gt;03.07.2022</t>
+  </si>
+  <si>
+    <t>Der komplette Rodalbener Felsenwanderweg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mit Übernachtung auf dem Hilschberghaus.&lt;br&gt;ca. 23 km je Tag, ca. 500 HM. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmeldung erforderlich bis 18.05.2022. </t>
+  </si>
+  <si>
+    <t>20220702_SPW_Rodalben_VORANKUENDIGUNG.pdf</t>
+  </si>
+  <si>
+    <t>Übernachtungswunsch: ________(Doppel/Dreifach/Einzelzimmer)</t>
+  </si>
+  <si>
+    <t>Auf dem Felsenwanderweg in Rodalben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW: ca. 11 km, KW: ca. 7 km. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treffpunkt: ab 09:00 Uhr an den üblichen Bushaltestellen. &lt;br&gt;Anmeldung erforderlich bis 22.06.2022. </t>
+  </si>
+  <si>
+    <t>20220703_MON_Rodalben.pdf</t>
+  </si>
+  <si>
+    <t>Radtour um den Hockenheimring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca. 40 km. </t>
+  </si>
+  <si>
+    <t>Fr-So&lt;br&gt;15.-17.&lt;br&gt;07.2022</t>
+  </si>
+  <si>
+    <t>Familienwochenende im Hochschwarzwald</t>
+  </si>
+  <si>
+    <t>in der JH Todtnauberg mit 2 Übernachtungen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmeldung erforderlich bis 09.06.2022. </t>
+  </si>
+  <si>
+    <t>20220715_FAM_Todtnauberg.pdf</t>
+  </si>
+  <si>
+    <t>Zum Schifferstadter Mittellacheweiher</t>
+  </si>
+  <si>
+    <t>N. N.</t>
+  </si>
+  <si>
+    <t>Barfußwandern in Rodalben mit der OG Landau</t>
+  </si>
+  <si>
+    <t>Auf den Spuren der Leininger Nonnen und Mönche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca. 15 km, ca. 450 HM. </t>
+  </si>
+  <si>
+    <t>Zur Eisenbahnbrücke nach Germersheim</t>
+  </si>
+  <si>
+    <t>Bach und Wiese: Heiderundweg Mehlingen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW: ca. 12 km, KW: ca. 7 km. </t>
+  </si>
+  <si>
+    <t>Roswitha Petry&lt;br&gt;Mechthild Porten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vom Forsthaus Heldenstein zum NFH Lambrecht im Kohlbachtal und zurück. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anreise mit dem Bus.&lt;br&gt;ca.12 km. </t>
+  </si>
+  <si>
+    <t>Erna Heck&lt;br&gt;Dieter Ofer</t>
+  </si>
+  <si>
+    <t>Rund um Burrweiler und Weyher – Fantastische Aussichten am Haardtrand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca. 18 km, ca. 850 HM. </t>
+  </si>
+  <si>
+    <t>Zu den Festungsanlagen in Germersheim</t>
+  </si>
+  <si>
+    <t>Infostand auf dem Speyerer Sattelfest</t>
+  </si>
+  <si>
+    <t>Große Runde auf dem Speyerer Sattelfest</t>
+  </si>
+  <si>
+    <t>Mit Triftknecht Johann unterwegs am Legelbach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW: ca. 10 km, KW: ca. 5 km. </t>
+  </si>
+  <si>
+    <t>Jungseniorenwanderung</t>
+  </si>
+  <si>
+    <t>Details zur Wanderung werden im Juli veröffentlicht.</t>
+  </si>
+  <si>
+    <t>Pony-Wanderung</t>
+  </si>
+  <si>
+    <t>Details zur Tour werden im Juli veröffentlicht.</t>
+  </si>
+  <si>
+    <t>Bizarre Felsen und atemberaubende Aussichten im Dahner Felsenland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca. 13 km, ca. 400 HM. </t>
+  </si>
+  <si>
+    <t>Ausflug in den Karlsruher Zoo</t>
+  </si>
+  <si>
     <t xml:space="preserve">ca. 5 km. </t>
   </si>
   <si>
-    <t>Mitgliederversammlung (Nachholtermin)</t>
+    <t>Monatstreffen Oktober</t>
+  </si>
+  <si>
+    <t>u. a Vorstellung der eingegangenen Wandervorschläge.</t>
   </si>
   <si>
     <t xml:space="preserve">Treffpunkt: 17:00 Uhr, Vereinsheim Skiclub Speyer. </t>
   </si>
   <si>
-    <t>Zur Rebenblüte durch die Deidesheimer Weinlagen</t>
-  </si>
-  <si>
-    <t>LW: ca. 11 km, KW: ca. 7 km.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auf der Ketscher Insel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anreise mit dem Rad, ca. 25 km.&lt;br&gt;8 km Wanderung. </t>
-  </si>
-  <si>
-    <t>Kinderspaß im Modenbachtal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treffpunkt: 11:00 Uhr, Stadthalle Speyer. &lt;br&gt;Anmeldefrist: 16.06.2022. </t>
-  </si>
-  <si>
-    <t>Sebastian Bittmann</t>
-  </si>
-  <si>
-    <t>20220619_FAM_Modenbachtal.pdf</t>
-  </si>
-  <si>
-    <t>Über Dudenhofen, Schifferstadt nach Waldsee und zurück</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ca. 28 km. </t>
-  </si>
-  <si>
-    <t>Wolfgang Laser</t>
-  </si>
-  <si>
-    <t>Sportliche Radwanderung von Speyer über Mussbach nach Deidesheim und zurück</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ca. 56 km. </t>
-  </si>
-  <si>
-    <t>Marcus Homa, Helmut Back</t>
-  </si>
-  <si>
-    <t>Barfußwandern auf die Rietburg mit der OG Landau</t>
-  </si>
-  <si>
-    <t>RAD-B</t>
-  </si>
-  <si>
-    <t>STADTRADELN PWV-Tour, Woche 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details werden noch bekanntgegeben.&lt;br&gt;ca. . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treffpunkt: 17:00 Uhr, Am Domnapf. </t>
-  </si>
-  <si>
-    <t>Sa / So&lt;br&gt;02.07.2022&lt;br&gt;03.07.2022</t>
-  </si>
-  <si>
-    <t>Der komplette Rodalbener Felsenwanderweg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mit Übernachtung auf dem Hilschberghaus..&lt;br&gt;ca. 23 km je Tag, ca. 500 HM. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anmeldefrist: 18.05.2022. </t>
-  </si>
-  <si>
-    <t>20220702_SPW_Rodalben_VORANKUENDIGUNG.pdf</t>
-  </si>
-  <si>
-    <t>Übernachtungswunsch: ________(Doppel/Dreifach/Einzelzimmer)</t>
-  </si>
-  <si>
-    <t>Auf dem Felsenwanderweg in Rodalben</t>
-  </si>
-  <si>
-    <t>Radtour um den Hockenheimring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ca. 40 km. </t>
-  </si>
-  <si>
-    <t>Fr-So&lt;br&gt;15.-17.&lt;br&gt;07.2022</t>
-  </si>
-  <si>
-    <t>Familienwochenende im Hochschwarzwald</t>
-  </si>
-  <si>
-    <t>in der JH Todtnauberg mit 2 Übernachtungen.&lt;br&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anmeldefrist: 09.06.2022. </t>
-  </si>
-  <si>
-    <t>20220715_FAM_Todtnauberg.pdf</t>
-  </si>
-  <si>
-    <t>Zum Schifferstadter Mittellacheweiher</t>
-  </si>
-  <si>
-    <t>N. N.</t>
-  </si>
-  <si>
-    <t>Barfußwandern in Rodalben mit der OG Landau</t>
-  </si>
-  <si>
-    <t>Auf den Spuren der Leininger Nonnen und Mönche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ca. 15 km, ca. 450 HM. </t>
-  </si>
-  <si>
-    <t>Zur Eisenbahnbrücke nach Germersheim</t>
-  </si>
-  <si>
-    <t>Bach und Wiese: Heiderundweg Mehlingen</t>
-  </si>
-  <si>
-    <t>LW: ca. 12 km, KW: ca. 7 km.</t>
-  </si>
-  <si>
-    <t>Roswitha Petry&lt;br&gt;Mechthild Porten</t>
-  </si>
-  <si>
-    <t>Wanderung wird im Juli veröffentlicht</t>
-  </si>
-  <si>
-    <t>Rund um Burrweiler und Weyher – Fantastische Aussichten am Haardtrand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ca. 18 km, ca. 850 HM. </t>
-  </si>
-  <si>
-    <t>Zu den Festungsanlagen in Germersheim</t>
-  </si>
-  <si>
-    <t>Infostand auf dem Speyerer Sattelfest</t>
-  </si>
-  <si>
-    <t>Große Runde auf dem Speyerer Sattelfest</t>
-  </si>
-  <si>
-    <t>Mit Triftknecht Johann unterwegs am Legelbach</t>
-  </si>
-  <si>
-    <t>LW: ca. 10 km, KW: ca. 5 km.</t>
-  </si>
-  <si>
-    <t>Jungseniorenwanderung</t>
-  </si>
-  <si>
-    <t>Details zur Wanderung werden im Juli veröffentlicht.&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>Pony-Wanderung</t>
-  </si>
-  <si>
-    <t>Details zur Tour werden im Juli veröffentlicht.&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>Bizarre Felsen und atemberaubende Aussichten im Dahner Felsenland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ca. 13 km, ca. 400 HM. </t>
-  </si>
-  <si>
-    <t>Ausflug in den Karlsruher Zoo</t>
-  </si>
-  <si>
-    <t>Monatstreffen Oktober</t>
-  </si>
-  <si>
-    <t>u. a Vorstellung der eingegangenen Wandervorschläge.&lt;br&gt;</t>
-  </si>
-  <si>
     <t>Hüttendienst auf der Böchinger Hütte</t>
   </si>
   <si>
@@ -687,7 +728,7 @@
     <t>Monatstreffen November</t>
   </si>
   <si>
-    <t>u. a. Vorstellung des vorläufigen Wanderplans 2023.&lt;br&gt;</t>
+    <t>u. a. Vorstellung des vorläufigen Wanderplans 2023.</t>
   </si>
   <si>
     <t>Max-Slevogt-Weg mit Trifels</t>
@@ -708,7 +749,7 @@
     <t>Zur Burg Falkenstein im Donnersberger Land</t>
   </si>
   <si>
-    <t>LW: ca. 14 km, KW: ca. 7 km.</t>
+    <t xml:space="preserve">LW: ca. 14 km, KW: ca. 7 km. </t>
   </si>
   <si>
     <t>Adventsfeier</t>
@@ -1238,15 +1279,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB255A1-6C92-48F2-848B-53EFDC97120D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794170E5-5F1E-47A2-A218-BA45C12CF8E9}">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,7 +1297,7 @@
     <col min="3" max="3" width="11.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39" style="2" customWidth="1"/>
     <col min="7" max="8" width="24.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="70.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.88671875" style="3" bestFit="1" customWidth="1"/>
@@ -1986,7 +2027,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>44699</v>
       </c>
@@ -1999,20 +2040,17 @@
       <c r="E32" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="I32" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="L32" s="5">
         <v>44697</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>44700</v>
       </c>
@@ -2025,9 +2063,6 @@
       <c r="E33" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="G33" s="3" t="s">
         <v>114</v>
       </c>
@@ -2038,7 +2073,7 @@
         <v>44684</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>44703</v>
       </c>
@@ -2046,28 +2081,25 @@
         <v>18</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="H34" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="I34" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="L34" s="5">
-        <v>44702</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>44709</v>
       </c>
@@ -2075,25 +2107,28 @@
         <v>68</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>54</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L35" s="5">
         <v>44707</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="M35" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>44716</v>
       </c>
@@ -2101,25 +2136,25 @@
         <v>34</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>54</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L36" s="5">
         <v>44714</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M36" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>44720</v>
       </c>
@@ -2127,17 +2162,25 @@
         <v>39</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L37" s="5"/>
-    </row>
-    <row r="38" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I37" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="L37" s="5">
+        <v>44718</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>44722</v>
       </c>
@@ -2145,17 +2188,14 @@
         <v>14</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>16</v>
       </c>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>44724</v>
       </c>
@@ -2163,17 +2203,28 @@
         <v>18</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L39" s="5"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H39" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="L39" s="5">
+        <v>44719</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>44727</v>
       </c>
@@ -2181,17 +2232,25 @@
         <v>29</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>151</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L40" s="5"/>
-    </row>
-    <row r="41" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="I40" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L40" s="5">
+        <v>44725</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>44731</v>
       </c>
@@ -2199,22 +2258,22 @@
         <v>24</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="L41" s="5">
         <v>44728</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>44734</v>
       </c>
@@ -2222,17 +2281,25 @@
         <v>116</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="L42" s="5"/>
-    </row>
-    <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L42" s="5">
+        <v>44732</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>44737</v>
       </c>
@@ -2240,17 +2307,25 @@
         <v>116</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="L43" s="5"/>
-    </row>
-    <row r="44" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L43" s="5">
+        <v>44735</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>44738</v>
       </c>
@@ -2258,67 +2333,83 @@
         <v>68</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="L44" s="5"/>
-    </row>
-    <row r="45" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I44" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="L44" s="5">
+        <v>44735</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44742</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L45" s="5"/>
-    </row>
-    <row r="46" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I45" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="L45" s="5">
+        <v>44740</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>44744</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="L46" s="5">
         <v>44699</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>44745</v>
       </c>
@@ -2326,17 +2417,25 @@
         <v>18</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>149</v>
+        <v>181</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L47" s="5"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I47" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="L47" s="5">
+        <v>44734</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>44751</v>
       </c>
@@ -2344,40 +2443,40 @@
         <v>116</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>54</v>
       </c>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>44757</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>27</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="L49" s="5">
         <v>44721</v>
@@ -2391,13 +2490,13 @@
         <v>29</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>125</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="L50" s="5"/>
     </row>
@@ -2409,7 +2508,7 @@
         <v>68</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>114</v>
@@ -2424,10 +2523,10 @@
         <v>34</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>21</v>
@@ -2442,10 +2541,10 @@
         <v>116</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>32</v>
@@ -2460,20 +2559,20 @@
         <v>18</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>44797</v>
       </c>
@@ -2481,7 +2580,13 @@
         <v>29</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>190</v>
+        <v>200</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="L55" s="5"/>
     </row>
@@ -2493,10 +2598,10 @@
         <v>34</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>37</v>
@@ -2511,7 +2616,7 @@
         <v>39</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>113</v>
@@ -2529,7 +2634,7 @@
         <v>68</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>54</v>
@@ -2544,10 +2649,10 @@
         <v>116</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>114</v>
@@ -2562,10 +2667,10 @@
         <v>18</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>32</v>
@@ -2580,10 +2685,10 @@
         <v>29</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="L61" s="5"/>
     </row>
@@ -2595,10 +2700,10 @@
         <v>24</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>54</v>
@@ -2613,10 +2718,10 @@
         <v>34</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>21</v>
@@ -2631,17 +2736,17 @@
         <v>39</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>44841</v>
       </c>
@@ -2649,13 +2754,13 @@
         <v>14</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>147</v>
+        <v>220</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>16</v>
@@ -2670,10 +2775,10 @@
         <v>29</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="L66" s="5"/>
     </row>
@@ -2685,7 +2790,7 @@
         <v>68</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>54</v>
@@ -2700,16 +2805,16 @@
         <v>18</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="L68" s="5"/>
     </row>
@@ -2721,7 +2826,7 @@
         <v>68</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>32</v>
@@ -2736,14 +2841,14 @@
         <v>24</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>54</v>
       </c>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>44869</v>
       </c>
@@ -2751,13 +2856,13 @@
         <v>14</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>147</v>
+        <v>220</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>16</v>
@@ -2772,10 +2877,10 @@
         <v>34</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>37</v>
@@ -2790,10 +2895,10 @@
         <v>39</v>
       </c>
       <c r="D73" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>59</v>
@@ -2808,10 +2913,10 @@
         <v>24</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="L74" s="5"/>
     </row>
@@ -2823,10 +2928,10 @@
         <v>18</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>32</v>
@@ -2844,14 +2949,14 @@
         <v>29</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>44898</v>
       </c>
@@ -2859,10 +2964,10 @@
         <v>14</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>16</v>
@@ -2874,13 +2979,13 @@
         <v>44901</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>32</v>
@@ -2895,7 +3000,7 @@
         <v>39</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="G79" s="3" t="s">
         <v>32</v>

</xml_diff>